<commit_message>
Updating for Jan 2021 EDI day. NOTE: Need to check down-correction!
</commit_message>
<xml_diff>
--- a/Data/DataAlreadyUploadedToEDI/EDIProductionFiles/MakeEMLInflow/Jan2021/20210104_RatingCurve.xlsx
+++ b/Data/DataAlreadyUploadedToEDI/EDIProductionFiles/MakeEMLInflow/Jan2021/20210104_RatingCurve.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoun\Desktop\Reservoirs\Data\DataAlreadyUploadedToEDI\EDIProductionFiles\MakeEMLInflow\Jan2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{69E062D1-347C-4052-A097-1E628BE26940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766C64AF-B848-49B4-B516-DA7404A3722E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20210104_RatingCurve" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>Pic_File_Name</t>
   </si>
@@ -218,14 +218,20 @@
   </si>
   <si>
     <t>Moved pressure transducers on 2 Sep 2020: 2 Sep 2020 - Present</t>
+  </si>
+  <si>
+    <t>07_Jan_21</t>
+  </si>
+  <si>
+    <t>FLAG: MAY NEED TO UPDATE IF WE REMOVE THE DOWN-CORRECTION!!!!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -734,13 +740,13 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -954,7 +960,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$G$3:$G$18</c:f>
+              <c:f>'20210104_RatingCurve'!$G$5:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1011,7 +1017,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$D$3:$D$18</c:f>
+              <c:f>'20210104_RatingCurve'!$D$5:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1153,7 +1159,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$H$3:$H$22</c:f>
+              <c:f>'20210104_RatingCurve'!$H$5:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1222,7 +1228,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$D$3:$D$22</c:f>
+              <c:f>'20210104_RatingCurve'!$D$5:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1751,7 +1757,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$G$35:$G$36</c:f>
+              <c:f>'20210104_RatingCurve'!$G$37:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1766,7 +1772,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$D$35:$D$36</c:f>
+              <c:f>'20210104_RatingCurve'!$D$37:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1866,7 +1872,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$H$35:$H$36</c:f>
+              <c:f>'20210104_RatingCurve'!$H$37:$H$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1881,7 +1887,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$D$35:$D$36</c:f>
+              <c:f>'20210104_RatingCurve'!$D$37:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2356,7 +2362,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$G$47:$G$57</c:f>
+              <c:f>'20210104_RatingCurve'!$G$49:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2369,8 +2375,20 @@
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.01</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4.4999999999999998E-2</c:v>
@@ -2380,7 +2398,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$D$47:$D$57</c:f>
+              <c:f>'20210104_RatingCurve'!$D$49:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2507,7 +2525,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$H$47:$H$57</c:f>
+              <c:f>'20210104_RatingCurve'!$H$49:$H$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2549,7 +2567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20210104_RatingCurve'!$D$47:$D$57</c:f>
+              <c:f>'20210104_RatingCurve'!$D$49:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4570,13 +4588,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>12382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>4855845</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>37147</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4606,13 +4624,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>116205</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>25717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>4684395</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>48577</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4642,13 +4660,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>110490</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>88582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>4676775</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>113347</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4973,11 +4991,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4993,122 +5012,69 @@
     <col min="9" max="9" width="84.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43626</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.4680555555555555</v>
-      </c>
-      <c r="D3">
-        <v>22.5</v>
-      </c>
-      <c r="E3">
-        <v>14.252000000000001</v>
-      </c>
-      <c r="F3">
-        <v>13.894</v>
-      </c>
-      <c r="G3">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="H3">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43640</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.53888888888888886</v>
-      </c>
-      <c r="D4">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>14.103999999999999</v>
-      </c>
-      <c r="F4">
-        <v>13.85</v>
-      </c>
-      <c r="G4">
-        <v>0.254</v>
-      </c>
-      <c r="H4">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>43643</v>
+        <v>43626</v>
       </c>
       <c r="C5" s="2">
-        <v>0.65902777777777777</v>
+        <v>0.4680555555555555</v>
       </c>
       <c r="D5">
-        <v>14.9</v>
+        <v>22.5</v>
       </c>
       <c r="E5">
-        <v>14.231</v>
+        <v>14.252000000000001</v>
       </c>
       <c r="F5">
-        <v>13.984</v>
+        <v>13.894</v>
       </c>
       <c r="G5">
-        <v>0.247</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="H5">
-        <v>0.29099999999999998</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -5116,28 +5082,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>43654</v>
+        <v>43640</v>
       </c>
       <c r="C6" s="2">
-        <v>0.57500000000000007</v>
+        <v>0.53888888888888886</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>14.061999999999999</v>
+        <v>14.103999999999999</v>
       </c>
       <c r="F6">
-        <v>13.904</v>
+        <v>13.85</v>
       </c>
       <c r="G6">
-        <v>0.158</v>
+        <v>0.254</v>
       </c>
       <c r="H6">
-        <v>0.253</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -5145,28 +5111,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>43668</v>
+        <v>43643</v>
       </c>
       <c r="C7" s="2">
-        <v>0.59652777777777777</v>
+        <v>0.65902777777777777</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>14.9</v>
       </c>
       <c r="E7">
-        <v>14.045999999999999</v>
+        <v>14.231</v>
       </c>
       <c r="F7">
-        <v>13.887</v>
+        <v>13.984</v>
       </c>
       <c r="G7">
-        <v>0.159</v>
+        <v>0.247</v>
       </c>
       <c r="H7">
-        <v>0.23200000000000001</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -5174,28 +5140,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>43689</v>
+        <v>43654</v>
       </c>
       <c r="C8" s="2">
-        <v>0.55625000000000002</v>
+        <v>0.57500000000000007</v>
       </c>
       <c r="D8">
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>14.112</v>
+        <v>14.061999999999999</v>
       </c>
       <c r="F8">
-        <v>13.925000000000001</v>
+        <v>13.904</v>
       </c>
       <c r="G8">
-        <v>0.187</v>
+        <v>0.158</v>
       </c>
       <c r="H8">
-        <v>0.25600000000000001</v>
+        <v>0.253</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
@@ -5203,28 +5169,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>43705</v>
+        <v>43668</v>
       </c>
       <c r="C9" s="2">
-        <v>0.68333333333333324</v>
+        <v>0.59652777777777777</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9">
-        <v>14.02</v>
+        <v>14.045999999999999</v>
       </c>
       <c r="F9">
-        <v>13.874000000000001</v>
+        <v>13.887</v>
       </c>
       <c r="G9">
-        <v>0.14599999999999999</v>
+        <v>0.159</v>
       </c>
       <c r="H9">
-        <v>0.221</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -5232,28 +5198,28 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>43735</v>
+        <v>43689</v>
       </c>
       <c r="C10" s="2">
-        <v>0.62013888888888891</v>
+        <v>0.55625000000000002</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>12.5</v>
       </c>
       <c r="E10">
-        <v>14.069000000000001</v>
+        <v>14.112</v>
       </c>
       <c r="F10">
-        <v>13.929</v>
+        <v>13.925000000000001</v>
       </c>
       <c r="G10">
-        <v>0.14000000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="H10">
-        <v>0.19600000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -5261,28 +5227,28 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>43768</v>
+        <v>43705</v>
       </c>
       <c r="C11" s="2">
-        <v>0.53888888888888886</v>
+        <v>0.68333333333333324</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>14.137</v>
+        <v>14.02</v>
       </c>
       <c r="F11">
-        <v>13.978</v>
+        <v>13.874000000000001</v>
       </c>
       <c r="G11">
-        <v>0.159</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="H11">
-        <v>0.222</v>
+        <v>0.221</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
@@ -5290,277 +5256,277 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
-        <v>43805</v>
+        <v>43735</v>
       </c>
       <c r="C12" s="2">
-        <v>0.5180555555555556</v>
+        <v>0.62013888888888891</v>
       </c>
       <c r="D12">
-        <v>13.5</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>14.166</v>
+        <v>14.069000000000001</v>
       </c>
       <c r="F12">
-        <v>13.95</v>
+        <v>13.929</v>
       </c>
       <c r="G12">
-        <v>0.216</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H12">
-        <v>0.22500000000000001</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
-        <v>43890</v>
+        <v>43768</v>
       </c>
       <c r="C13" s="2">
-        <v>0.47916666666666669</v>
+        <v>0.53888888888888886</v>
       </c>
       <c r="D13">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>13.888</v>
+        <v>14.137</v>
       </c>
       <c r="F13">
-        <v>14.069000000000001</v>
+        <v>13.978</v>
       </c>
       <c r="G13">
-        <v>0.18099999999999999</v>
+        <v>0.159</v>
       </c>
       <c r="H13">
-        <v>0.23</v>
+        <v>0.222</v>
       </c>
       <c r="I13" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>43914</v>
+        <v>43805</v>
       </c>
       <c r="C14" s="2">
-        <v>0.53125</v>
+        <v>0.5180555555555556</v>
       </c>
       <c r="D14">
-        <v>10.5</v>
+        <v>13.5</v>
       </c>
       <c r="E14">
-        <v>13.923999999999999</v>
+        <v>14.166</v>
       </c>
       <c r="F14">
-        <v>14.11</v>
+        <v>13.95</v>
       </c>
       <c r="G14">
-        <v>0.186</v>
+        <v>0.216</v>
       </c>
       <c r="H14">
-        <v>0.24099999999999999</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
-        <v>43920</v>
+        <v>43890</v>
       </c>
       <c r="C15" s="2">
-        <v>0.73125000000000007</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D15">
         <v>10.5</v>
       </c>
       <c r="E15">
-        <v>13.836</v>
+        <v>13.888</v>
       </c>
       <c r="F15">
-        <v>14.02</v>
+        <v>14.069000000000001</v>
       </c>
       <c r="G15">
-        <v>0.184</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="H15">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="I15" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
-        <v>43941</v>
+        <v>43914</v>
       </c>
       <c r="C16" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.53125</v>
       </c>
       <c r="D16">
-        <v>25</v>
+        <v>10.5</v>
       </c>
       <c r="E16">
-        <v>13.724</v>
+        <v>13.923999999999999</v>
       </c>
       <c r="F16">
-        <v>14.103</v>
+        <v>14.11</v>
       </c>
       <c r="G16">
-        <v>0.379</v>
+        <v>0.186</v>
       </c>
       <c r="H16">
-        <v>0.43099999999999999</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
-        <v>43943</v>
+        <v>43920</v>
       </c>
       <c r="C17" s="2">
-        <v>0.5229166666666667</v>
+        <v>0.73125000000000007</v>
       </c>
       <c r="D17">
-        <v>22.2</v>
+        <v>10.5</v>
       </c>
       <c r="E17">
-        <v>13.894</v>
+        <v>13.836</v>
       </c>
       <c r="F17">
-        <v>14.236000000000001</v>
+        <v>14.02</v>
       </c>
       <c r="G17">
-        <v>0.34200000000000003</v>
+        <v>0.184</v>
       </c>
       <c r="H17">
-        <v>0.39500000000000002</v>
+        <v>0.24</v>
       </c>
       <c r="I17" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
-        <v>43962</v>
+        <v>43941</v>
       </c>
       <c r="C18" s="2">
-        <v>0.62638888888888888</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D18">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E18">
-        <v>13.906000000000001</v>
+        <v>13.724</v>
       </c>
       <c r="F18">
-        <v>14.239000000000001</v>
+        <v>14.103</v>
       </c>
       <c r="G18">
-        <v>0.33300000000000002</v>
+        <v>0.379</v>
       </c>
       <c r="H18">
-        <v>0.38200000000000001</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="I18" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1">
-        <v>43969</v>
+        <v>43943</v>
       </c>
       <c r="C19" s="2">
-        <v>0.52013888888888882</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="D19">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
+        <v>22.2</v>
+      </c>
+      <c r="E19">
+        <v>13.894</v>
+      </c>
+      <c r="F19">
+        <v>14.236000000000001</v>
+      </c>
+      <c r="G19">
+        <v>0.34200000000000003</v>
       </c>
       <c r="H19">
-        <v>0.34399999999999997</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1">
-        <v>43976</v>
+        <v>43962</v>
       </c>
       <c r="C20" s="2">
-        <v>0.57500000000000007</v>
+        <v>0.62638888888888888</v>
       </c>
       <c r="D20">
-        <v>30</v>
-      </c>
-      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20">
+        <v>13.906000000000001</v>
+      </c>
+      <c r="F20">
+        <v>14.239000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="H20">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="I20" t="s">
         <v>10</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="I20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1">
-        <v>43994</v>
+        <v>43969</v>
       </c>
       <c r="C21" s="2">
-        <v>0.55208333333333337</v>
+        <v>0.52013888888888882</v>
       </c>
       <c r="D21">
-        <v>28.5</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -5572,422 +5538,431 @@
         <v>10</v>
       </c>
       <c r="H21">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="I21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43976</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43994</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D23">
+        <v>28.5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
         <v>0.47799999999999998</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B24" s="7">
         <v>44018</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C24" s="8">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D24" s="6">
         <v>28</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H24" s="6">
         <v>0.47</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I24" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+    <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+    <row r="28" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
         <v>27.5</v>
       </c>
-      <c r="B26" s="11">
-        <f>(A26+0.6479)/65.436</f>
+      <c r="B28" s="11">
+        <f>(A28+0.6479)/65.436</f>
         <v>0.43015923956232038</v>
       </c>
-      <c r="C26" s="11">
-        <f>(A26+5.6633)/70.64</f>
+      <c r="C28" s="11">
+        <f>(A28+5.6633)/70.64</f>
         <v>0.46946913929784823</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+    <row r="29" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C31" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
+    <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
         <v>0</v>
       </c>
-      <c r="B30" s="11">
-        <f>(A30+0.6479)/65.436</f>
+      <c r="B32" s="11">
+        <f>(A32+0.6479)/65.436</f>
         <v>9.9012775842044123E-3</v>
       </c>
-      <c r="C30" s="11">
-        <f>(A30+5.6633)/70.64</f>
+      <c r="C32" s="11">
+        <f>(A32+5.6633)/70.64</f>
         <v>8.0171291053227622E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1">
-        <v>44053</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="1">
-        <v>44056</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" t="s">
-        <v>40</v>
-      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44053</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44056</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B37" s="1">
         <v>44067</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C37" s="2">
         <v>0.65694444444444444</v>
       </c>
-      <c r="D35">
+      <c r="D37">
         <v>12</v>
       </c>
-      <c r="E35">
+      <c r="E37">
         <v>13.923</v>
       </c>
-      <c r="F35">
+      <c r="F37">
         <v>14.032</v>
       </c>
-      <c r="G35">
+      <c r="G37">
         <v>0.109</v>
       </c>
-      <c r="H35">
+      <c r="H37">
         <v>0.156</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+    <row r="38" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B38" s="7">
         <v>44076</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C38" s="8">
         <v>0.58888888888888891</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D38" s="6">
         <v>14.5</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E38" s="6">
         <v>13.858000000000001</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F38" s="6">
         <v>14.012</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G38" s="6">
         <v>0.154</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H38" s="10">
         <v>0.2</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I38" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+    <row r="39" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B41" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6">
+    <row r="42" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
         <v>27.5</v>
       </c>
-      <c r="B40" s="11">
-        <f>(A40-5.9444)/55.556</f>
+      <c r="B42" s="11">
+        <f>(A42-5.9444)/55.556</f>
         <v>0.38799769601843181</v>
       </c>
-      <c r="C40" s="11">
-        <f>(A40-3.1364)/56.818</f>
+      <c r="C42" s="11">
+        <f>(A42-3.1364)/56.818</f>
         <v>0.42880073216234288</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="42" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-    </row>
-    <row r="43" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C45" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6">
+    <row r="46" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
         <v>0</v>
       </c>
-      <c r="B44" s="11">
-        <f>(A44-5.9444)/55.556</f>
+      <c r="B46" s="11">
+        <f>(A46-5.9444)/55.556</f>
         <v>-0.1069983440132479</v>
       </c>
-      <c r="C44" s="11">
-        <f>(A44-3.1364)/56.818</f>
+      <c r="C46" s="11">
+        <f>(A46-3.1364)/56.818</f>
         <v>-5.5200816642613261E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
+    <row r="47" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="7"/>
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B49" s="7">
         <v>44076</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C49" s="8">
         <v>0.6118055555555556</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D49" s="6">
         <v>14.5</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E49" s="6">
         <v>13.847</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F49" s="6">
         <v>13.909000000000001</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G49" s="6">
         <v>6.2E-2</v>
       </c>
-      <c r="H47" s="10">
+      <c r="H49" s="10">
         <v>0.109</v>
       </c>
-      <c r="I47" s="6" t="s">
+      <c r="I49" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="1">
-        <v>44083</v>
-      </c>
-      <c r="C48" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="D48">
-        <v>10</v>
-      </c>
-      <c r="E48">
-        <v>14</v>
-      </c>
-      <c r="F48">
-        <v>14</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="I48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="1">
-        <v>44087</v>
-      </c>
-      <c r="C49" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D49">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="E49">
-        <v>13.964</v>
-      </c>
-      <c r="F49">
-        <v>13.964</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I49" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1">
-        <v>44089</v>
+        <v>44083</v>
       </c>
       <c r="C50" s="2">
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D50">
         <v>10</v>
       </c>
+      <c r="E50">
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <v>14</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
       <c r="H50">
-        <v>4.5999999999999999E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="I50" t="s">
         <v>24</v>
@@ -5995,19 +5970,28 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1">
-        <v>44090</v>
+        <v>44087</v>
       </c>
       <c r="C51" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E51">
+        <v>13.964</v>
+      </c>
+      <c r="F51">
+        <v>13.964</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>4.8000000000000001E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="I51" t="s">
         <v>24</v>
@@ -6015,28 +5999,28 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1">
-        <v>44104</v>
+        <v>44089</v>
       </c>
       <c r="C52" s="2">
-        <v>0.55694444444444446</v>
+        <v>0.625</v>
       </c>
       <c r="D52">
-        <v>12.8</v>
+        <v>10</v>
       </c>
       <c r="E52">
-        <v>13.855</v>
+        <v>14.016</v>
       </c>
       <c r="F52">
-        <v>13.875999999999999</v>
+        <v>14.004</v>
       </c>
       <c r="G52">
-        <v>2.1000000000000001E-2</v>
+        <v>-1.2E-2</v>
       </c>
       <c r="H52">
-        <v>8.1000000000000003E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="I52" t="s">
         <v>24</v>
@@ -6044,19 +6028,28 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1">
-        <v>44109</v>
+        <v>44090</v>
       </c>
       <c r="C53" s="2">
-        <v>0.65069444444444446</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D53">
         <v>10</v>
       </c>
+      <c r="E53">
+        <v>13.962999999999999</v>
+      </c>
+      <c r="F53">
+        <v>13.952999999999999</v>
+      </c>
+      <c r="G53">
+        <v>-0.01</v>
+      </c>
       <c r="H53">
-        <v>4.2999999999999997E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="I53" t="s">
         <v>24</v>
@@ -6064,19 +6057,28 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1">
-        <v>44123</v>
+        <v>44104</v>
       </c>
       <c r="C54" s="2">
-        <v>0.6875</v>
+        <v>0.55694444444444446</v>
       </c>
       <c r="D54">
-        <v>10</v>
+        <v>12.8</v>
+      </c>
+      <c r="E54">
+        <v>13.855</v>
+      </c>
+      <c r="F54">
+        <v>13.875999999999999</v>
+      </c>
+      <c r="G54">
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H54">
-        <v>4.4999999999999998E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="I54" t="s">
         <v>24</v>
@@ -6084,48 +6086,57 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1">
-        <v>44137</v>
+        <v>44109</v>
       </c>
       <c r="C55" s="2">
-        <v>0.54722222222222217</v>
+        <v>0.65069444444444446</v>
       </c>
       <c r="D55">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E55">
-        <v>13.974</v>
+        <v>13.967000000000001</v>
       </c>
       <c r="F55">
-        <v>14.019</v>
+        <v>13.944000000000001</v>
       </c>
       <c r="G55">
-        <v>4.4999999999999998E-2</v>
+        <v>-2.3E-2</v>
       </c>
       <c r="H55">
-        <v>0.106</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I55" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1">
-        <v>44144</v>
+        <v>44123</v>
       </c>
       <c r="C56" s="2">
-        <v>0.55138888888888882</v>
+        <v>0.6875</v>
       </c>
       <c r="D56">
-        <v>11.3</v>
+        <v>10</v>
+      </c>
+      <c r="E56">
+        <v>13.922000000000001</v>
+      </c>
+      <c r="F56">
+        <v>13.974</v>
+      </c>
+      <c r="G56">
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="H56">
-        <v>5.7000000000000002E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I56" t="s">
         <v>24</v>
@@ -6133,79 +6144,142 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B57" s="1">
-        <v>44192</v>
+        <v>44137</v>
       </c>
       <c r="C57" s="2">
-        <v>0.55208333333333337</v>
+        <v>0.54722222222222217</v>
       </c>
       <c r="D57">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="E57">
+        <v>13.974</v>
+      </c>
+      <c r="F57">
+        <v>14.019</v>
+      </c>
+      <c r="G57">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="H57">
-        <v>0.20100000000000001</v>
+        <v>0.106</v>
       </c>
       <c r="I57" t="s">
-        <v>56</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="1">
+        <v>44144</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.55138888888888882</v>
+      </c>
+      <c r="D58">
+        <v>11.3</v>
+      </c>
+      <c r="H58">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I58" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="B59" s="1">
+        <v>44192</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D59">
+        <v>23</v>
+      </c>
+      <c r="H59">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I59" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>27.5</v>
-      </c>
-      <c r="B61" s="17">
-        <f>(A61-10.451)/80.047</f>
-        <v>0.21298736992017189</v>
-      </c>
-      <c r="C61" s="17">
-        <f>(A61-6.0386)/83.285</f>
-        <v>0.25768625802965722</v>
+        <v>66</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44203</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>27.5</v>
+      </c>
+      <c r="B64" s="17">
+        <f>(A64-10.451)/80.047</f>
+        <v>0.21298736992017189</v>
+      </c>
+      <c r="C64" s="17">
+        <f>(A64-6.0386)/83.285</f>
+        <v>0.25768625802965722</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>59</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>60</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C67" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>0</v>
       </c>
-      <c r="B65" s="17">
-        <f>(A65-10.451)/80.047</f>
+      <c r="B68" s="17">
+        <f>(A68-10.451)/80.047</f>
         <v>-0.13056079553262459</v>
       </c>
-      <c r="C65" s="17">
-        <f>(A65-6.0386)/83.285</f>
+      <c r="C68" s="17">
+        <f>(A68-6.0386)/83.285</f>
         <v>-7.2505253046767124E-2</v>
       </c>
     </row>

</xml_diff>